<commit_message>
found an open source color palette
</commit_message>
<xml_diff>
--- a/TestData/original.xlsx
+++ b/TestData/original.xlsx
@@ -1212,7 +1212,7 @@
           <t>QC Comments</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AB1" s="0" t="inlineStr">
         <is>
           <t>Unnamed: 27</t>
         </is>
@@ -1241,7 +1241,7 @@
           <t>Edison Illuminating Companies proceedings on alternating current</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="0" t="n">
         <v/>
       </c>
       <c r="H2" s="18" t="inlineStr">
@@ -1326,7 +1326,7 @@
           <t>Extent (10) does not match page count (11)</t>
         </is>
       </c>
-      <c r="AB2" t="n">
+      <c r="AB2" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -1353,7 +1353,7 @@
           <t>Transformer pamphlets</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="0" t="n">
         <v/>
       </c>
       <c r="H3" s="18" t="inlineStr">
@@ -1439,10 +1439,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA3" t="n">
-        <v/>
-      </c>
-      <c r="AB3" t="n">
+      <c r="AA3" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB3" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -1469,7 +1469,7 @@
           <t>Transformer pamphlets</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="0" t="n">
         <v/>
       </c>
       <c r="H4" s="18" t="inlineStr">
@@ -1555,10 +1555,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA4" t="n">
-        <v/>
-      </c>
-      <c r="AB4" t="n">
+      <c r="AA4" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB4" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -1585,7 +1585,7 @@
           <t>Cornell University Report on Stanley Transformer</t>
         </is>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="0" t="n">
         <v/>
       </c>
       <c r="H5" s="18" t="inlineStr">
@@ -1671,10 +1671,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA5" t="n">
-        <v/>
-      </c>
-      <c r="AB5" t="n">
+      <c r="AA5" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB5" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -1701,7 +1701,7 @@
           <t>"Apparatus for Transmission of Light and Power by Two Phase Alternating Currents</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="0" t="n">
         <v/>
       </c>
       <c r="H6" s="18" t="inlineStr">
@@ -1787,10 +1787,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA6" t="n">
-        <v/>
-      </c>
-      <c r="AB6" t="n">
+      <c r="AA6" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB6" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -1817,7 +1817,7 @@
           <t>"Apparatus for Transmission of Light and Power by Two Phase Alternating Currents</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="0" t="n">
         <v/>
       </c>
       <c r="H7" s="18" t="inlineStr">
@@ -1935,7 +1935,7 @@
           <t>S.K.C. booklet</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="0" t="n">
         <v/>
       </c>
       <c r="H8" s="18" t="inlineStr">
@@ -2019,10 +2019,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA8" t="n">
-        <v/>
-      </c>
-      <c r="AB8" t="n">
+      <c r="AA8" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB8" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2049,7 +2049,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="0" t="n">
         <v/>
       </c>
       <c r="H9" s="18" t="inlineStr">
@@ -2131,10 +2131,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA9" t="n">
-        <v/>
-      </c>
-      <c r="AB9" t="n">
+      <c r="AA9" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB9" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2161,7 +2161,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="0" t="n">
         <v/>
       </c>
       <c r="H10" s="18" t="inlineStr">
@@ -2243,10 +2243,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA10" t="n">
-        <v/>
-      </c>
-      <c r="AB10" t="n">
+      <c r="AA10" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB10" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2273,7 +2273,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="G11" s="0" t="n">
         <v/>
       </c>
       <c r="H11" s="18" t="inlineStr">
@@ -2355,10 +2355,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA11" t="n">
-        <v/>
-      </c>
-      <c r="AB11" t="n">
+      <c r="AA11" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB11" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2385,7 +2385,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="G12" s="0" t="n">
         <v/>
       </c>
       <c r="H12" s="18" t="inlineStr">
@@ -2472,7 +2472,7 @@
           <t>Page 8 cropping looks off</t>
         </is>
       </c>
-      <c r="AB12" t="n">
+      <c r="AB12" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2499,7 +2499,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" s="0" t="n">
         <v/>
       </c>
       <c r="H13" s="18" t="inlineStr">
@@ -2581,10 +2581,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA13" t="n">
-        <v/>
-      </c>
-      <c r="AB13" t="n">
+      <c r="AA13" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB13" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G14" t="n">
+      <c r="G14" s="0" t="n">
         <v/>
       </c>
       <c r="H14" s="18" t="inlineStr">
@@ -2693,10 +2693,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA14" t="n">
-        <v/>
-      </c>
-      <c r="AB14" t="n">
+      <c r="AA14" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB14" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2723,7 +2723,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="G15" s="0" t="n">
         <v/>
       </c>
       <c r="H15" s="18" t="inlineStr">
@@ -2805,10 +2805,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA15" t="n">
-        <v/>
-      </c>
-      <c r="AB15" t="n">
+      <c r="AA15" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB15" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2835,7 +2835,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G16" t="n">
+      <c r="G16" s="0" t="n">
         <v/>
       </c>
       <c r="H16" s="18" t="inlineStr">
@@ -2917,10 +2917,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA16" t="n">
-        <v/>
-      </c>
-      <c r="AB16" t="n">
+      <c r="AA16" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB16" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -2947,7 +2947,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="G17" s="0" t="n">
         <v/>
       </c>
       <c r="H17" s="18" t="inlineStr">
@@ -3029,10 +3029,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA17" t="n">
-        <v/>
-      </c>
-      <c r="AB17" t="n">
+      <c r="AA17" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB17" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3059,7 +3059,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="G18" s="0" t="n">
         <v/>
       </c>
       <c r="H18" s="18" t="inlineStr">
@@ -3141,10 +3141,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA18" t="n">
-        <v/>
-      </c>
-      <c r="AB18" t="n">
+      <c r="AA18" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB18" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3171,7 +3171,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="G19" s="0" t="n">
         <v/>
       </c>
       <c r="H19" s="18" t="inlineStr">
@@ -3253,10 +3253,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA19" t="n">
-        <v/>
-      </c>
-      <c r="AB19" t="n">
+      <c r="AA19" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB19" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3283,7 +3283,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" s="0" t="n">
         <v/>
       </c>
       <c r="H20" s="18" t="inlineStr">
@@ -3363,10 +3363,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA20" t="n">
-        <v/>
-      </c>
-      <c r="AB20" t="n">
+      <c r="AA20" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB20" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3393,7 +3393,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G21" t="n">
+      <c r="G21" s="0" t="n">
         <v/>
       </c>
       <c r="H21" s="18" t="inlineStr">
@@ -3473,10 +3473,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA21" t="n">
-        <v/>
-      </c>
-      <c r="AB21" t="n">
+      <c r="AA21" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB21" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3503,7 +3503,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G22" t="n">
+      <c r="G22" s="0" t="n">
         <v/>
       </c>
       <c r="H22" s="18" t="inlineStr">
@@ -3585,10 +3585,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA22" t="n">
-        <v/>
-      </c>
-      <c r="AB22" t="n">
+      <c r="AA22" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB22" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3615,7 +3615,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G23" t="n">
+      <c r="G23" s="0" t="n">
         <v/>
       </c>
       <c r="H23" s="18" t="inlineStr">
@@ -3697,10 +3697,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA23" t="n">
-        <v/>
-      </c>
-      <c r="AB23" t="n">
+      <c r="AA23" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB23" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3727,7 +3727,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G24" t="n">
+      <c r="G24" s="0" t="n">
         <v/>
       </c>
       <c r="H24" s="18" t="inlineStr">
@@ -3809,10 +3809,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA24" t="n">
-        <v/>
-      </c>
-      <c r="AB24" t="n">
+      <c r="AA24" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB24" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3839,7 +3839,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G25" t="n">
+      <c r="G25" s="0" t="n">
         <v/>
       </c>
       <c r="H25" s="18" t="inlineStr">
@@ -3921,10 +3921,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA25" t="n">
-        <v/>
-      </c>
-      <c r="AB25" t="n">
+      <c r="AA25" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB25" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -3951,7 +3951,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G26" t="n">
+      <c r="G26" s="0" t="n">
         <v/>
       </c>
       <c r="H26" s="18" t="inlineStr">
@@ -4033,10 +4033,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA26" t="n">
-        <v/>
-      </c>
-      <c r="AB26" t="n">
+      <c r="AA26" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB26" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4063,7 +4063,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G27" t="n">
+      <c r="G27" s="0" t="n">
         <v/>
       </c>
       <c r="H27" s="18" t="inlineStr">
@@ -4145,10 +4145,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA27" t="n">
-        <v/>
-      </c>
-      <c r="AB27" t="n">
+      <c r="AA27" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB27" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4175,7 +4175,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G28" t="n">
+      <c r="G28" s="0" t="n">
         <v/>
       </c>
       <c r="H28" s="18" t="inlineStr">
@@ -4257,10 +4257,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA28" t="n">
-        <v/>
-      </c>
-      <c r="AB28" t="n">
+      <c r="AA28" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB28" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4287,7 +4287,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G29" t="n">
+      <c r="G29" s="0" t="n">
         <v/>
       </c>
       <c r="H29" s="18" t="inlineStr">
@@ -4369,10 +4369,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA29" t="n">
-        <v/>
-      </c>
-      <c r="AB29" t="n">
+      <c r="AA29" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB29" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4399,7 +4399,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G30" t="n">
+      <c r="G30" s="0" t="n">
         <v/>
       </c>
       <c r="H30" s="18" t="inlineStr">
@@ -4481,10 +4481,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA30" t="n">
-        <v/>
-      </c>
-      <c r="AB30" t="n">
+      <c r="AA30" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB30" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4511,7 +4511,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G31" t="n">
+      <c r="G31" s="0" t="n">
         <v/>
       </c>
       <c r="H31" s="18" t="inlineStr">
@@ -4593,10 +4593,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA31" t="n">
-        <v/>
-      </c>
-      <c r="AB31" t="n">
+      <c r="AA31" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB31" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4623,7 +4623,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G32" t="n">
+      <c r="G32" s="0" t="n">
         <v/>
       </c>
       <c r="H32" s="18" t="inlineStr">
@@ -4705,10 +4705,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA32" t="n">
-        <v/>
-      </c>
-      <c r="AB32" t="n">
+      <c r="AA32" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB32" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4735,7 +4735,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G33" t="n">
+      <c r="G33" s="0" t="n">
         <v/>
       </c>
       <c r="H33" s="18" t="inlineStr">
@@ -4817,10 +4817,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA33" t="n">
-        <v/>
-      </c>
-      <c r="AB33" t="n">
+      <c r="AA33" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB33" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4847,7 +4847,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G34" t="n">
+      <c r="G34" s="0" t="n">
         <v/>
       </c>
       <c r="H34" s="18" t="inlineStr">
@@ -4929,10 +4929,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA34" t="n">
-        <v/>
-      </c>
-      <c r="AB34" t="n">
+      <c r="AA34" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB34" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -4959,7 +4959,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G35" t="n">
+      <c r="G35" s="0" t="n">
         <v/>
       </c>
       <c r="H35" s="18" t="inlineStr">
@@ -5041,10 +5041,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA35" t="n">
-        <v/>
-      </c>
-      <c r="AB35" t="n">
+      <c r="AA35" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB35" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5071,7 +5071,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G36" t="n">
+      <c r="G36" s="0" t="n">
         <v/>
       </c>
       <c r="H36" s="18" t="inlineStr">
@@ -5148,7 +5148,7 @@
           <t>Fail Corrected</t>
         </is>
       </c>
-      <c r="Z36" t="n">
+      <c r="Z36" s="0" t="n">
         <v/>
       </c>
       <c r="AA36" s="103" t="inlineStr">
@@ -5156,7 +5156,7 @@
           <t xml:space="preserve">RESCAN </t>
         </is>
       </c>
-      <c r="AB36" t="n">
+      <c r="AB36" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5183,7 +5183,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G37" t="n">
+      <c r="G37" s="0" t="n">
         <v/>
       </c>
       <c r="H37" s="18" t="inlineStr">
@@ -5265,10 +5265,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA37" t="n">
-        <v/>
-      </c>
-      <c r="AB37" t="n">
+      <c r="AA37" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB37" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5295,7 +5295,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G38" t="n">
+      <c r="G38" s="0" t="n">
         <v/>
       </c>
       <c r="H38" s="18" t="inlineStr">
@@ -5375,10 +5375,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA38" t="n">
-        <v/>
-      </c>
-      <c r="AB38" t="n">
+      <c r="AA38" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB38" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5405,7 +5405,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G39" t="n">
+      <c r="G39" s="0" t="n">
         <v/>
       </c>
       <c r="H39" s="18" t="inlineStr">
@@ -5492,7 +5492,7 @@
           <t>Extent does not match (spreadsheet says 8 pages, there are 9 on the scan)</t>
         </is>
       </c>
-      <c r="AB39" t="n">
+      <c r="AB39" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5519,7 +5519,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G40" t="n">
+      <c r="G40" s="0" t="n">
         <v/>
       </c>
       <c r="H40" s="18" t="inlineStr">
@@ -5601,10 +5601,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA40" t="n">
-        <v/>
-      </c>
-      <c r="AB40" t="n">
+      <c r="AA40" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB40" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5631,7 +5631,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G41" t="n">
+      <c r="G41" s="0" t="n">
         <v/>
       </c>
       <c r="H41" s="18" t="inlineStr">
@@ -5713,10 +5713,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA41" t="n">
-        <v/>
-      </c>
-      <c r="AB41" t="n">
+      <c r="AA41" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB41" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5743,7 +5743,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G42" t="n">
+      <c r="G42" s="0" t="n">
         <v/>
       </c>
       <c r="H42" s="18" t="inlineStr">
@@ -5825,10 +5825,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA42" t="n">
-        <v/>
-      </c>
-      <c r="AB42" t="n">
+      <c r="AA42" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB42" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5855,7 +5855,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G43" t="n">
+      <c r="G43" s="0" t="n">
         <v/>
       </c>
       <c r="H43" s="18" t="inlineStr">
@@ -5937,10 +5937,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA43" t="n">
-        <v/>
-      </c>
-      <c r="AB43" t="n">
+      <c r="AA43" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB43" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -5967,7 +5967,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G44" t="n">
+      <c r="G44" s="0" t="n">
         <v/>
       </c>
       <c r="H44" s="18" t="inlineStr">
@@ -6049,10 +6049,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA44" t="n">
-        <v/>
-      </c>
-      <c r="AB44" t="n">
+      <c r="AA44" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB44" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6079,7 +6079,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G45" t="n">
+      <c r="G45" s="0" t="n">
         <v/>
       </c>
       <c r="H45" s="18" t="inlineStr">
@@ -6161,10 +6161,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA45" t="n">
-        <v/>
-      </c>
-      <c r="AB45" t="n">
+      <c r="AA45" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB45" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6191,7 +6191,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G46" t="n">
+      <c r="G46" s="0" t="n">
         <v/>
       </c>
       <c r="H46" s="18" t="inlineStr">
@@ -6273,10 +6273,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA46" t="n">
-        <v/>
-      </c>
-      <c r="AB46" t="n">
+      <c r="AA46" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB46" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6303,7 +6303,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G47" t="n">
+      <c r="G47" s="0" t="n">
         <v/>
       </c>
       <c r="H47" s="18" t="inlineStr">
@@ -6385,10 +6385,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA47" t="n">
-        <v/>
-      </c>
-      <c r="AB47" t="n">
+      <c r="AA47" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB47" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6415,7 +6415,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G48" t="n">
+      <c r="G48" s="0" t="n">
         <v/>
       </c>
       <c r="H48" s="18" t="inlineStr">
@@ -6497,10 +6497,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA48" t="n">
-        <v/>
-      </c>
-      <c r="AB48" t="n">
+      <c r="AA48" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB48" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6527,7 +6527,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G49" t="n">
+      <c r="G49" s="0" t="n">
         <v/>
       </c>
       <c r="H49" s="18" t="inlineStr">
@@ -6609,10 +6609,10 @@
           <t>RB</t>
         </is>
       </c>
-      <c r="AA49" t="n">
-        <v/>
-      </c>
-      <c r="AB49" t="n">
+      <c r="AA49" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB49" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6639,7 +6639,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G50" t="n">
+      <c r="G50" s="0" t="n">
         <v/>
       </c>
       <c r="H50" s="18" t="inlineStr">
@@ -6721,10 +6721,10 @@
           <t>GH</t>
         </is>
       </c>
-      <c r="AA50" t="n">
-        <v/>
-      </c>
-      <c r="AB50" t="n">
+      <c r="AA50" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB50" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6751,7 +6751,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G51" t="n">
+      <c r="G51" s="0" t="n">
         <v/>
       </c>
       <c r="H51" s="18" t="inlineStr">
@@ -6833,10 +6833,10 @@
           <t>GH</t>
         </is>
       </c>
-      <c r="AA51" t="n">
-        <v/>
-      </c>
-      <c r="AB51" t="n">
+      <c r="AA51" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB51" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6863,7 +6863,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G52" t="n">
+      <c r="G52" s="0" t="n">
         <v/>
       </c>
       <c r="H52" s="18" t="inlineStr">
@@ -6950,7 +6950,7 @@
           <t>Page 11 looks a little sideways</t>
         </is>
       </c>
-      <c r="AB52" t="n">
+      <c r="AB52" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -6977,7 +6977,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G53" t="n">
+      <c r="G53" s="0" t="n">
         <v/>
       </c>
       <c r="H53" s="18" t="inlineStr">
@@ -7059,10 +7059,10 @@
           <t>GH</t>
         </is>
       </c>
-      <c r="AA53" t="n">
-        <v/>
-      </c>
-      <c r="AB53" t="n">
+      <c r="AA53" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB53" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -7089,7 +7089,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G54" t="n">
+      <c r="G54" s="0" t="n">
         <v/>
       </c>
       <c r="H54" s="18" t="inlineStr">
@@ -7171,10 +7171,10 @@
           <t>GH</t>
         </is>
       </c>
-      <c r="AA54" t="n">
-        <v/>
-      </c>
-      <c r="AB54" t="n">
+      <c r="AA54" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB54" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -7201,7 +7201,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G55" t="n">
+      <c r="G55" s="0" t="n">
         <v/>
       </c>
       <c r="H55" s="18" t="inlineStr">
@@ -7283,10 +7283,10 @@
           <t>MW</t>
         </is>
       </c>
-      <c r="AA55" t="n">
-        <v/>
-      </c>
-      <c r="AB55" t="n">
+      <c r="AA55" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB55" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -7313,7 +7313,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G56" t="n">
+      <c r="G56" s="0" t="n">
         <v/>
       </c>
       <c r="H56" s="18" t="inlineStr">
@@ -7395,10 +7395,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA56" t="n">
-        <v/>
-      </c>
-      <c r="AB56" t="n">
+      <c r="AA56" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB56" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -7425,7 +7425,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G57" t="n">
+      <c r="G57" s="0" t="n">
         <v/>
       </c>
       <c r="H57" s="18" t="inlineStr">
@@ -7507,10 +7507,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA57" t="n">
-        <v/>
-      </c>
-      <c r="AB57" t="n">
+      <c r="AA57" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB57" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -7537,7 +7537,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G58" t="n">
+      <c r="G58" s="0" t="n">
         <v/>
       </c>
       <c r="H58" s="18" t="inlineStr">
@@ -7619,10 +7619,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA58" t="n">
-        <v/>
-      </c>
-      <c r="AB58" t="n">
+      <c r="AA58" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB58" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -7649,7 +7649,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G59" t="n">
+      <c r="G59" s="0" t="n">
         <v/>
       </c>
       <c r="H59" s="18" t="inlineStr">
@@ -7731,7 +7731,7 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA59" t="n">
+      <c r="AA59" s="0" t="n">
         <v/>
       </c>
       <c r="AB59" s="103" t="inlineStr">
@@ -7763,7 +7763,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G60" t="n">
+      <c r="G60" s="0" t="n">
         <v/>
       </c>
       <c r="H60" s="18" t="inlineStr">
@@ -7771,13 +7771,13 @@
           <t>Stanley Electric Manufacturing Company, Engineering Bulletin, No. 6</t>
         </is>
       </c>
-      <c r="I60" t="n">
-        <v/>
-      </c>
-      <c r="J60" t="n">
-        <v/>
-      </c>
-      <c r="K60" t="n">
+      <c r="I60" s="0" t="n">
+        <v/>
+      </c>
+      <c r="J60" s="0" t="n">
+        <v/>
+      </c>
+      <c r="K60" s="0" t="n">
         <v/>
       </c>
       <c r="L60" s="18" t="n">
@@ -7841,7 +7841,7 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA60" t="n">
+      <c r="AA60" s="0" t="n">
         <v/>
       </c>
       <c r="AB60" s="103" t="inlineStr">
@@ -7873,7 +7873,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G61" t="n">
+      <c r="G61" s="0" t="n">
         <v/>
       </c>
       <c r="H61" s="18" t="inlineStr">
@@ -7955,7 +7955,7 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA61" t="n">
+      <c r="AA61" s="0" t="n">
         <v/>
       </c>
       <c r="AB61" s="103" t="inlineStr">
@@ -7987,7 +7987,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G62" t="n">
+      <c r="G62" s="0" t="n">
         <v/>
       </c>
       <c r="H62" s="18" t="inlineStr">
@@ -8069,7 +8069,7 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA62" t="n">
+      <c r="AA62" s="0" t="n">
         <v/>
       </c>
       <c r="AB62" s="103" t="n">
@@ -8099,7 +8099,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G63" t="n">
+      <c r="G63" s="0" t="n">
         <v/>
       </c>
       <c r="H63" s="18" t="inlineStr">
@@ -8181,7 +8181,7 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA63" t="n">
+      <c r="AA63" s="0" t="n">
         <v/>
       </c>
       <c r="AB63" s="103" t="inlineStr">
@@ -8213,7 +8213,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G64" t="n">
+      <c r="G64" s="0" t="n">
         <v/>
       </c>
       <c r="H64" s="18" t="inlineStr">
@@ -8295,10 +8295,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA64" t="n">
-        <v/>
-      </c>
-      <c r="AB64" t="n">
+      <c r="AA64" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB64" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -8325,7 +8325,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G65" t="n">
+      <c r="G65" s="0" t="n">
         <v/>
       </c>
       <c r="H65" s="18" t="inlineStr">
@@ -8407,7 +8407,7 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA65" t="n">
+      <c r="AA65" s="0" t="n">
         <v/>
       </c>
       <c r="AB65" s="16" t="inlineStr">
@@ -8439,7 +8439,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G66" t="n">
+      <c r="G66" s="0" t="n">
         <v/>
       </c>
       <c r="H66" s="18" t="inlineStr">
@@ -8519,10 +8519,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA66" t="n">
-        <v/>
-      </c>
-      <c r="AB66" t="n">
+      <c r="AA66" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB66" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -8549,7 +8549,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G67" t="n">
+      <c r="G67" s="0" t="n">
         <v/>
       </c>
       <c r="H67" s="18" t="inlineStr">
@@ -8631,10 +8631,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA67" t="n">
-        <v/>
-      </c>
-      <c r="AB67" t="n">
+      <c r="AA67" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB67" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -8661,7 +8661,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G68" t="n">
+      <c r="G68" s="0" t="n">
         <v/>
       </c>
       <c r="H68" s="18" t="inlineStr">
@@ -8743,10 +8743,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA68" t="n">
-        <v/>
-      </c>
-      <c r="AB68" t="n">
+      <c r="AA68" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB68" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -8773,7 +8773,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G69" t="n">
+      <c r="G69" s="0" t="n">
         <v/>
       </c>
       <c r="H69" s="18" t="inlineStr">
@@ -8855,10 +8855,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA69" t="n">
-        <v/>
-      </c>
-      <c r="AB69" t="n">
+      <c r="AA69" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB69" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -8885,7 +8885,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G70" t="n">
+      <c r="G70" s="0" t="n">
         <v/>
       </c>
       <c r="H70" s="18" t="inlineStr">
@@ -8972,7 +8972,7 @@
           <t>Color looks off/greenish</t>
         </is>
       </c>
-      <c r="AB70" t="n">
+      <c r="AB70" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -8999,7 +8999,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G71" t="n">
+      <c r="G71" s="0" t="n">
         <v/>
       </c>
       <c r="H71" s="18" t="inlineStr">
@@ -9086,7 +9086,7 @@
           <t>Color looks off/reddish</t>
         </is>
       </c>
-      <c r="AB71" t="n">
+      <c r="AB71" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -9113,7 +9113,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G72" t="n">
+      <c r="G72" s="0" t="n">
         <v/>
       </c>
       <c r="H72" s="18" t="inlineStr">
@@ -9200,7 +9200,7 @@
           <t>Page 11 needs deskew</t>
         </is>
       </c>
-      <c r="AB72" t="n">
+      <c r="AB72" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -9227,7 +9227,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G73" t="n">
+      <c r="G73" s="0" t="n">
         <v/>
       </c>
       <c r="H73" s="18" t="inlineStr">
@@ -9309,10 +9309,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA73" t="n">
-        <v/>
-      </c>
-      <c r="AB73" t="n">
+      <c r="AA73" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB73" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -9339,7 +9339,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G74" t="n">
+      <c r="G74" s="0" t="n">
         <v/>
       </c>
       <c r="H74" s="18" t="inlineStr">
@@ -9421,10 +9421,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA74" t="n">
-        <v/>
-      </c>
-      <c r="AB74" t="n">
+      <c r="AA74" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB74" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -9451,7 +9451,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G75" t="n">
+      <c r="G75" s="0" t="n">
         <v/>
       </c>
       <c r="H75" s="18" t="inlineStr">
@@ -9538,7 +9538,7 @@
           <t>Extent doesn't match page #</t>
         </is>
       </c>
-      <c r="AB75" t="n">
+      <c r="AB75" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -9565,7 +9565,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G76" t="n">
+      <c r="G76" s="0" t="n">
         <v/>
       </c>
       <c r="H76" s="18" t="inlineStr">
@@ -9652,7 +9652,7 @@
           <t>Can't find file in sharepoint - Found (RF)</t>
         </is>
       </c>
-      <c r="AB76" t="n">
+      <c r="AB76" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -9679,7 +9679,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G77" t="n">
+      <c r="G77" s="0" t="n">
         <v/>
       </c>
       <c r="H77" s="18" t="inlineStr">
@@ -9766,7 +9766,7 @@
           <t>Cropping is off on some of the pages</t>
         </is>
       </c>
-      <c r="AB77" t="n">
+      <c r="AB77" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -9793,7 +9793,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G78" t="n">
+      <c r="G78" s="0" t="n">
         <v/>
       </c>
       <c r="H78" s="18" t="inlineStr">
@@ -9880,7 +9880,7 @@
           <t>Page 1 needs deskew</t>
         </is>
       </c>
-      <c r="AB78" t="n">
+      <c r="AB78" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -9907,7 +9907,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G79" t="n">
+      <c r="G79" s="0" t="n">
         <v/>
       </c>
       <c r="H79" s="18" t="inlineStr">
@@ -9989,10 +9989,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA79" t="n">
-        <v/>
-      </c>
-      <c r="AB79" t="n">
+      <c r="AA79" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB79" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10019,7 +10019,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G80" t="n">
+      <c r="G80" s="0" t="n">
         <v/>
       </c>
       <c r="H80" s="18" t="inlineStr">
@@ -10101,10 +10101,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA80" t="n">
-        <v/>
-      </c>
-      <c r="AB80" t="n">
+      <c r="AA80" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB80" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10131,7 +10131,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G81" t="n">
+      <c r="G81" s="0" t="n">
         <v/>
       </c>
       <c r="H81" s="18" t="inlineStr">
@@ -10213,10 +10213,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA81" t="n">
-        <v/>
-      </c>
-      <c r="AB81" t="n">
+      <c r="AA81" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB81" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10243,7 +10243,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G82" t="n">
+      <c r="G82" s="0" t="n">
         <v/>
       </c>
       <c r="H82" s="18" t="inlineStr">
@@ -10325,10 +10325,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA82" t="n">
-        <v/>
-      </c>
-      <c r="AB82" t="n">
+      <c r="AA82" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB82" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10355,7 +10355,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G83" t="n">
+      <c r="G83" s="0" t="n">
         <v/>
       </c>
       <c r="H83" s="18" t="inlineStr">
@@ -10437,10 +10437,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA83" t="n">
-        <v/>
-      </c>
-      <c r="AB83" t="n">
+      <c r="AA83" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB83" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10467,7 +10467,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G84" t="n">
+      <c r="G84" s="0" t="n">
         <v/>
       </c>
       <c r="H84" s="18" t="inlineStr">
@@ -10549,10 +10549,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA84" t="n">
-        <v/>
-      </c>
-      <c r="AB84" t="n">
+      <c r="AA84" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB84" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10579,7 +10579,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G85" t="n">
+      <c r="G85" s="0" t="n">
         <v/>
       </c>
       <c r="H85" s="18" t="inlineStr">
@@ -10661,10 +10661,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA85" t="n">
-        <v/>
-      </c>
-      <c r="AB85" t="n">
+      <c r="AA85" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB85" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10691,7 +10691,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G86" t="n">
+      <c r="G86" s="0" t="n">
         <v/>
       </c>
       <c r="H86" s="18" t="inlineStr">
@@ -10773,10 +10773,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA86" t="n">
-        <v/>
-      </c>
-      <c r="AB86" t="n">
+      <c r="AA86" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB86" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10803,7 +10803,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G87" t="n">
+      <c r="G87" s="0" t="n">
         <v/>
       </c>
       <c r="H87" s="18" t="inlineStr">
@@ -10885,10 +10885,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA87" t="n">
-        <v/>
-      </c>
-      <c r="AB87" t="n">
+      <c r="AA87" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB87" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -10915,7 +10915,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G88" t="n">
+      <c r="G88" s="0" t="n">
         <v/>
       </c>
       <c r="H88" s="18" t="inlineStr">
@@ -10997,10 +10997,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA88" t="n">
-        <v/>
-      </c>
-      <c r="AB88" t="n">
+      <c r="AA88" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB88" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11027,7 +11027,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G89" t="n">
+      <c r="G89" s="0" t="n">
         <v/>
       </c>
       <c r="H89" s="18" t="inlineStr">
@@ -11114,7 +11114,7 @@
           <t>Color is off/reddish</t>
         </is>
       </c>
-      <c r="AB89" t="n">
+      <c r="AB89" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11141,7 +11141,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G90" t="n">
+      <c r="G90" s="0" t="n">
         <v/>
       </c>
       <c r="H90" s="18" t="inlineStr">
@@ -11223,10 +11223,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA90" t="n">
-        <v/>
-      </c>
-      <c r="AB90" t="n">
+      <c r="AA90" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB90" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11253,7 +11253,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G91" t="n">
+      <c r="G91" s="0" t="n">
         <v/>
       </c>
       <c r="H91" s="18" t="inlineStr">
@@ -11335,10 +11335,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA91" t="n">
-        <v/>
-      </c>
-      <c r="AB91" t="n">
+      <c r="AA91" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB91" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11365,7 +11365,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G92" t="n">
+      <c r="G92" s="0" t="n">
         <v/>
       </c>
       <c r="H92" s="18" t="inlineStr">
@@ -11447,10 +11447,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA92" t="n">
-        <v/>
-      </c>
-      <c r="AB92" t="n">
+      <c r="AA92" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB92" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11477,7 +11477,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G93" t="n">
+      <c r="G93" s="0" t="n">
         <v/>
       </c>
       <c r="H93" s="18" t="inlineStr">
@@ -11559,10 +11559,10 @@
           <t>SG</t>
         </is>
       </c>
-      <c r="AA93" t="n">
-        <v/>
-      </c>
-      <c r="AB93" t="n">
+      <c r="AA93" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB93" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11589,7 +11589,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G94" t="n">
+      <c r="G94" s="0" t="n">
         <v/>
       </c>
       <c r="H94" s="18" t="inlineStr">
@@ -11671,10 +11671,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA94" t="n">
-        <v/>
-      </c>
-      <c r="AB94" t="n">
+      <c r="AA94" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB94" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11701,7 +11701,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G95" t="n">
+      <c r="G95" s="0" t="n">
         <v/>
       </c>
       <c r="H95" s="18" t="inlineStr">
@@ -11783,10 +11783,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA95" t="n">
-        <v/>
-      </c>
-      <c r="AB95" t="n">
+      <c r="AA95" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB95" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11813,7 +11813,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G96" t="n">
+      <c r="G96" s="0" t="n">
         <v/>
       </c>
       <c r="H96" s="18" t="inlineStr">
@@ -11895,10 +11895,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA96" t="n">
-        <v/>
-      </c>
-      <c r="AB96" t="n">
+      <c r="AA96" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB96" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -11925,7 +11925,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G97" t="n">
+      <c r="G97" s="0" t="n">
         <v/>
       </c>
       <c r="H97" s="18" t="inlineStr">
@@ -12007,10 +12007,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA97" t="n">
-        <v/>
-      </c>
-      <c r="AB97" t="n">
+      <c r="AA97" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB97" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -12037,7 +12037,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G98" t="n">
+      <c r="G98" s="0" t="n">
         <v/>
       </c>
       <c r="H98" s="18" t="inlineStr">
@@ -12119,10 +12119,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA98" t="n">
-        <v/>
-      </c>
-      <c r="AB98" t="n">
+      <c r="AA98" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB98" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -12264,7 +12264,7 @@
           <t>S.K.C. and engineering bulletins</t>
         </is>
       </c>
-      <c r="G100" t="n">
+      <c r="G100" s="0" t="n">
         <v/>
       </c>
       <c r="H100" s="18" t="inlineStr">
@@ -12344,10 +12344,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA100" t="n">
-        <v/>
-      </c>
-      <c r="AB100" t="n">
+      <c r="AA100" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB100" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -12374,7 +12374,7 @@
           <t>"Synopsis of the S.K.C. System"</t>
         </is>
       </c>
-      <c r="G101" t="n">
+      <c r="G101" s="0" t="n">
         <v/>
       </c>
       <c r="H101" s="18" t="inlineStr">
@@ -12456,10 +12456,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA101" t="n">
-        <v/>
-      </c>
-      <c r="AB101" t="n">
+      <c r="AA101" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB101" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -12486,7 +12486,7 @@
           <t>"Synopsis of the S.K.C. System"</t>
         </is>
       </c>
-      <c r="G102" t="n">
+      <c r="G102" s="0" t="n">
         <v/>
       </c>
       <c r="H102" s="18" t="inlineStr">
@@ -12568,10 +12568,10 @@
           <t>MC</t>
         </is>
       </c>
-      <c r="AA102" t="n">
-        <v/>
-      </c>
-      <c r="AB102" t="n">
+      <c r="AA102" s="0" t="n">
+        <v/>
+      </c>
+      <c r="AB102" s="0" t="n">
         <v/>
       </c>
     </row>
@@ -22905,7 +22905,7 @@
           <t>QC Comments</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AB1" s="0" t="inlineStr">
         <is>
           <t>Unnamed: 27</t>
         </is>
@@ -33386,7 +33386,7 @@
           <t>Can't find file</t>
         </is>
       </c>
-      <c r="AB93" t="n">
+      <c r="AB93" s="0" t="n">
         <v/>
       </c>
       <c r="AC93" s="68" t="n"/>
@@ -42686,7 +42686,7 @@
       <c r="Z3" s="68" t="n">
         <v/>
       </c>
-      <c r="AA3" t="n">
+      <c r="AA3" s="0" t="n">
         <v/>
       </c>
       <c r="AB3" s="103" t="n">
@@ -42802,7 +42802,7 @@
       <c r="Z4" s="68" t="n">
         <v/>
       </c>
-      <c r="AA4" t="n">
+      <c r="AA4" s="0" t="n">
         <v/>
       </c>
       <c r="AB4" s="103" t="n">
@@ -43160,7 +43160,7 @@
       <c r="Z7" s="68" t="n">
         <v/>
       </c>
-      <c r="AA7" t="n">
+      <c r="AA7" s="0" t="n">
         <v/>
       </c>
       <c r="AB7" s="103" t="n">
@@ -43276,7 +43276,7 @@
       <c r="Z8" s="68" t="n">
         <v/>
       </c>
-      <c r="AA8" t="n">
+      <c r="AA8" s="0" t="n">
         <v/>
       </c>
       <c r="AB8" s="103" t="n">
@@ -43394,7 +43394,7 @@
           <t>Original copy is tinted pink</t>
         </is>
       </c>
-      <c r="AA9" t="n">
+      <c r="AA9" s="0" t="n">
         <v/>
       </c>
       <c r="AB9" s="103" t="n">
@@ -43510,7 +43510,7 @@
       <c r="Z10" s="68" t="n">
         <v/>
       </c>
-      <c r="AA10" t="n">
+      <c r="AA10" s="0" t="n">
         <v/>
       </c>
       <c r="AB10" s="103" t="n">
@@ -43626,7 +43626,7 @@
       <c r="Z11" s="68" t="n">
         <v/>
       </c>
-      <c r="AA11" t="n">
+      <c r="AA11" s="0" t="n">
         <v/>
       </c>
       <c r="AB11" s="103" t="n">
@@ -43742,7 +43742,7 @@
       <c r="Z12" s="68" t="n">
         <v/>
       </c>
-      <c r="AA12" t="n">
+      <c r="AA12" s="0" t="n">
         <v/>
       </c>
       <c r="AB12" s="103" t="n">
@@ -43858,7 +43858,7 @@
       <c r="Z13" s="68" t="n">
         <v/>
       </c>
-      <c r="AA13" t="n">
+      <c r="AA13" s="0" t="n">
         <v/>
       </c>
       <c r="AB13" s="103" t="n">
@@ -43974,7 +43974,7 @@
       <c r="Z14" s="68" t="n">
         <v/>
       </c>
-      <c r="AA14" t="n">
+      <c r="AA14" s="0" t="n">
         <v/>
       </c>
       <c r="AB14" s="103" t="n">
@@ -44090,7 +44090,7 @@
       <c r="Z15" s="68" t="n">
         <v/>
       </c>
-      <c r="AA15" t="n">
+      <c r="AA15" s="0" t="n">
         <v/>
       </c>
       <c r="AB15" s="103" t="n">
@@ -44206,7 +44206,7 @@
       <c r="Z16" s="68" t="n">
         <v/>
       </c>
-      <c r="AA16" t="n">
+      <c r="AA16" s="0" t="n">
         <v/>
       </c>
       <c r="AB16" s="103" t="n">
@@ -44322,7 +44322,7 @@
       <c r="Z17" s="68" t="n">
         <v/>
       </c>
-      <c r="AA17" t="n">
+      <c r="AA17" s="0" t="n">
         <v/>
       </c>
       <c r="AB17" s="103" t="n">
@@ -44438,7 +44438,7 @@
       <c r="Z18" s="68" t="n">
         <v/>
       </c>
-      <c r="AA18" t="n">
+      <c r="AA18" s="0" t="n">
         <v/>
       </c>
       <c r="AB18" s="103" t="n">
@@ -44554,7 +44554,7 @@
       <c r="Z19" s="68" t="n">
         <v/>
       </c>
-      <c r="AA19" t="n">
+      <c r="AA19" s="0" t="n">
         <v/>
       </c>
       <c r="AB19" s="103" t="n">
@@ -44670,7 +44670,7 @@
       <c r="Z20" s="68" t="n">
         <v/>
       </c>
-      <c r="AA20" t="n">
+      <c r="AA20" s="0" t="n">
         <v/>
       </c>
       <c r="AB20" s="103" t="n">
@@ -44786,7 +44786,7 @@
       <c r="Z21" s="68" t="n">
         <v/>
       </c>
-      <c r="AA21" t="n">
+      <c r="AA21" s="0" t="n">
         <v/>
       </c>
       <c r="AB21" s="103" t="n">
@@ -44902,7 +44902,7 @@
       <c r="Z22" s="68" t="n">
         <v/>
       </c>
-      <c r="AA22" t="n">
+      <c r="AA22" s="0" t="n">
         <v/>
       </c>
       <c r="AB22" s="103" t="n">
@@ -45018,7 +45018,7 @@
       <c r="Z23" s="68" t="n">
         <v/>
       </c>
-      <c r="AA23" t="n">
+      <c r="AA23" s="0" t="n">
         <v/>
       </c>
       <c r="AB23" s="103" t="n">
@@ -45134,7 +45134,7 @@
       <c r="Z24" s="68" t="n">
         <v/>
       </c>
-      <c r="AA24" t="n">
+      <c r="AA24" s="0" t="n">
         <v/>
       </c>
       <c r="AB24" s="103" t="n">
@@ -45250,7 +45250,7 @@
       <c r="Z25" s="68" t="n">
         <v/>
       </c>
-      <c r="AA25" t="n">
+      <c r="AA25" s="0" t="n">
         <v/>
       </c>
       <c r="AB25" s="103" t="n">
@@ -45366,7 +45366,7 @@
       <c r="Z26" s="68" t="n">
         <v/>
       </c>
-      <c r="AA26" t="n">
+      <c r="AA26" s="0" t="n">
         <v/>
       </c>
       <c r="AB26" s="103" t="n">
@@ -45482,7 +45482,7 @@
       <c r="Z27" s="68" t="n">
         <v/>
       </c>
-      <c r="AA27" t="n">
+      <c r="AA27" s="0" t="n">
         <v/>
       </c>
       <c r="AB27" s="103" t="n">
@@ -45600,7 +45600,7 @@
           <t xml:space="preserve">Date earlier than listed on ASPACE - is that ok? </t>
         </is>
       </c>
-      <c r="AA28" t="n">
+      <c r="AA28" s="0" t="n">
         <v/>
       </c>
       <c r="AB28" s="103" t="n">
@@ -45716,7 +45716,7 @@
       <c r="Z29" s="68" t="n">
         <v/>
       </c>
-      <c r="AA29" t="n">
+      <c r="AA29" s="0" t="n">
         <v/>
       </c>
       <c r="AB29" s="103" t="n">
@@ -45834,7 +45834,7 @@
           <t>End of Right Side of Folder</t>
         </is>
       </c>
-      <c r="AA30" t="n">
+      <c r="AA30" s="0" t="n">
         <v/>
       </c>
       <c r="AB30" s="103" t="n">
@@ -45952,7 +45952,7 @@
           <t xml:space="preserve">Start of Left Side of Folder </t>
         </is>
       </c>
-      <c r="AA31" t="n">
+      <c r="AA31" s="0" t="n">
         <v/>
       </c>
       <c r="AB31" s="103" t="n">
@@ -46068,7 +46068,7 @@
       <c r="Z32" s="68" t="n">
         <v/>
       </c>
-      <c r="AA32" t="n">
+      <c r="AA32" s="0" t="n">
         <v/>
       </c>
       <c r="AB32" s="103" t="n">
@@ -46184,7 +46184,7 @@
       <c r="Z33" s="68" t="n">
         <v/>
       </c>
-      <c r="AA33" t="n">
+      <c r="AA33" s="0" t="n">
         <v/>
       </c>
       <c r="AB33" s="103" t="n">
@@ -46300,7 +46300,7 @@
       <c r="Z34" s="68" t="n">
         <v/>
       </c>
-      <c r="AA34" t="n">
+      <c r="AA34" s="0" t="n">
         <v/>
       </c>
       <c r="AB34" s="103" t="n">
@@ -46416,7 +46416,7 @@
       <c r="Z35" s="68" t="n">
         <v/>
       </c>
-      <c r="AA35" t="n">
+      <c r="AA35" s="0" t="n">
         <v/>
       </c>
       <c r="AB35" s="103" t="n">
@@ -46534,7 +46534,7 @@
       <c r="Z36" s="68" t="n">
         <v/>
       </c>
-      <c r="AA36" t="n">
+      <c r="AA36" s="0" t="n">
         <v/>
       </c>
       <c r="AB36" s="103" t="n">
@@ -46652,7 +46652,7 @@
       <c r="Z37" s="68" t="n">
         <v/>
       </c>
-      <c r="AA37" t="n">
+      <c r="AA37" s="0" t="n">
         <v/>
       </c>
       <c r="AB37" s="103" t="n">
@@ -46768,7 +46768,7 @@
       <c r="Z38" s="68" t="n">
         <v/>
       </c>
-      <c r="AA38" t="n">
+      <c r="AA38" s="0" t="n">
         <v/>
       </c>
       <c r="AB38" s="103" t="n">
@@ -46884,7 +46884,7 @@
       <c r="Z39" s="68" t="n">
         <v/>
       </c>
-      <c r="AA39" t="n">
+      <c r="AA39" s="0" t="n">
         <v/>
       </c>
       <c r="AB39" s="103" t="n">
@@ -48203,7 +48203,7 @@
           <t xml:space="preserve">Right side of the folder. </t>
         </is>
       </c>
-      <c r="AA50" t="n">
+      <c r="AA50" s="0" t="n">
         <v/>
       </c>
       <c r="AB50" s="43" t="inlineStr">
@@ -48321,7 +48321,7 @@
       <c r="Z51" s="68" t="n">
         <v/>
       </c>
-      <c r="AA51" t="n">
+      <c r="AA51" s="0" t="n">
         <v/>
       </c>
       <c r="AB51" s="43" t="inlineStr">
@@ -48680,7 +48680,7 @@
       <c r="Z54" s="68" t="n">
         <v/>
       </c>
-      <c r="AA54" t="n">
+      <c r="AA54" s="0" t="n">
         <v/>
       </c>
       <c r="AB54" s="103" t="n">
@@ -48796,7 +48796,7 @@
       <c r="Z55" s="68" t="n">
         <v/>
       </c>
-      <c r="AA55" t="n">
+      <c r="AA55" s="0" t="n">
         <v/>
       </c>
       <c r="AB55" s="103" t="n">
@@ -48912,7 +48912,7 @@
       <c r="Z56" s="68" t="n">
         <v/>
       </c>
-      <c r="AA56" t="n">
+      <c r="AA56" s="0" t="n">
         <v/>
       </c>
       <c r="AB56" s="103" t="n">
@@ -49028,7 +49028,7 @@
       <c r="Z57" s="68" t="n">
         <v/>
       </c>
-      <c r="AA57" t="n">
+      <c r="AA57" s="0" t="n">
         <v/>
       </c>
       <c r="AB57" s="103" t="n">
@@ -49144,7 +49144,7 @@
       <c r="Z58" s="68" t="n">
         <v/>
       </c>
-      <c r="AA58" t="n">
+      <c r="AA58" s="0" t="n">
         <v/>
       </c>
       <c r="AB58" s="103" t="n">
@@ -49260,7 +49260,7 @@
       <c r="Z59" s="68" t="n">
         <v/>
       </c>
-      <c r="AA59" t="n">
+      <c r="AA59" s="0" t="n">
         <v/>
       </c>
       <c r="AB59" s="103" t="n">
@@ -49495,7 +49495,7 @@
       <c r="Z61" s="68" t="n">
         <v/>
       </c>
-      <c r="AA61" t="n">
+      <c r="AA61" s="0" t="n">
         <v/>
       </c>
       <c r="AB61" s="103" t="n">
@@ -49730,7 +49730,7 @@
       <c r="Z63" s="68" t="n">
         <v/>
       </c>
-      <c r="AA63" t="n">
+      <c r="AA63" s="0" t="n">
         <v/>
       </c>
       <c r="AB63" s="103" t="n">
@@ -49846,7 +49846,7 @@
       <c r="Z64" s="68" t="n">
         <v/>
       </c>
-      <c r="AA64" t="n">
+      <c r="AA64" s="0" t="n">
         <v/>
       </c>
       <c r="AB64" s="103" t="n">
@@ -49962,7 +49962,7 @@
       <c r="Z65" s="68" t="n">
         <v/>
       </c>
-      <c r="AA65" t="n">
+      <c r="AA65" s="0" t="n">
         <v/>
       </c>
       <c r="AB65" s="103" t="n">
@@ -50078,7 +50078,7 @@
       <c r="Z66" s="68" t="n">
         <v/>
       </c>
-      <c r="AA66" t="n">
+      <c r="AA66" s="0" t="n">
         <v/>
       </c>
       <c r="AB66" s="103" t="n">
@@ -50194,7 +50194,7 @@
       <c r="Z67" s="68" t="n">
         <v/>
       </c>
-      <c r="AA67" t="n">
+      <c r="AA67" s="0" t="n">
         <v/>
       </c>
       <c r="AB67" s="103" t="n">
@@ -50429,7 +50429,7 @@
       <c r="Z69" s="68" t="n">
         <v/>
       </c>
-      <c r="AA69" t="n">
+      <c r="AA69" s="0" t="n">
         <v/>
       </c>
       <c r="AB69" s="103" t="n">
@@ -50666,7 +50666,7 @@
           <t xml:space="preserve">End of right side </t>
         </is>
       </c>
-      <c r="AA71" t="n">
+      <c r="AA71" s="0" t="n">
         <v/>
       </c>
       <c r="AB71" s="103" t="n">
@@ -50784,7 +50784,7 @@
           <t xml:space="preserve">start of left side </t>
         </is>
       </c>
-      <c r="AA72" t="n">
+      <c r="AA72" s="0" t="n">
         <v/>
       </c>
       <c r="AB72" s="103" t="n">
@@ -50900,7 +50900,7 @@
       <c r="Z73" s="68" t="n">
         <v/>
       </c>
-      <c r="AA73" t="n">
+      <c r="AA73" s="0" t="n">
         <v/>
       </c>
       <c r="AB73" s="103" t="n">
@@ -51016,7 +51016,7 @@
       <c r="Z74" s="68" t="n">
         <v/>
       </c>
-      <c r="AA74" t="n">
+      <c r="AA74" s="0" t="n">
         <v/>
       </c>
       <c r="AB74" s="103" t="n">
@@ -51132,7 +51132,7 @@
       <c r="Z75" s="68" t="n">
         <v/>
       </c>
-      <c r="AA75" t="n">
+      <c r="AA75" s="0" t="n">
         <v/>
       </c>
       <c r="AB75" s="103" t="n">
@@ -51248,7 +51248,7 @@
       <c r="Z76" s="68" t="n">
         <v/>
       </c>
-      <c r="AA76" t="n">
+      <c r="AA76" s="0" t="n">
         <v/>
       </c>
       <c r="AB76" s="103" t="n">
@@ -51364,7 +51364,7 @@
       <c r="Z77" s="68" t="n">
         <v/>
       </c>
-      <c r="AA77" t="n">
+      <c r="AA77" s="0" t="n">
         <v/>
       </c>
       <c r="AB77" s="103" t="n">
@@ -51480,7 +51480,7 @@
       <c r="Z78" s="68" t="n">
         <v/>
       </c>
-      <c r="AA78" t="n">
+      <c r="AA78" s="0" t="n">
         <v/>
       </c>
       <c r="AB78" s="103" t="n">
@@ -51715,7 +51715,7 @@
       <c r="Z80" s="68" t="n">
         <v/>
       </c>
-      <c r="AA80" t="n">
+      <c r="AA80" s="0" t="n">
         <v/>
       </c>
       <c r="AB80" s="103" t="n">
@@ -51831,7 +51831,7 @@
       <c r="Z81" s="68" t="n">
         <v/>
       </c>
-      <c r="AA81" t="n">
+      <c r="AA81" s="0" t="n">
         <v/>
       </c>
       <c r="AB81" s="103" t="n">
@@ -51947,7 +51947,7 @@
       <c r="Z82" s="68" t="n">
         <v/>
       </c>
-      <c r="AA82" t="n">
+      <c r="AA82" s="0" t="n">
         <v/>
       </c>
       <c r="AB82" s="103" t="n">
@@ -52063,7 +52063,7 @@
       <c r="Z83" s="68" t="n">
         <v/>
       </c>
-      <c r="AA83" t="n">
+      <c r="AA83" s="0" t="n">
         <v/>
       </c>
       <c r="AB83" s="103" t="n">
@@ -52179,7 +52179,7 @@
       <c r="Z84" s="68" t="n">
         <v/>
       </c>
-      <c r="AA84" t="n">
+      <c r="AA84" s="0" t="n">
         <v/>
       </c>
       <c r="AB84" s="103" t="n">
@@ -52414,7 +52414,7 @@
       <c r="Z86" s="68" t="n">
         <v/>
       </c>
-      <c r="AA86" t="n">
+      <c r="AA86" s="0" t="n">
         <v/>
       </c>
       <c r="AB86" s="103" t="n">
@@ -52530,7 +52530,7 @@
       <c r="Z87" s="68" t="n">
         <v/>
       </c>
-      <c r="AA87" t="n">
+      <c r="AA87" s="0" t="n">
         <v/>
       </c>
       <c r="AB87" s="103" t="n">
@@ -52648,7 +52648,7 @@
           <t xml:space="preserve">Date earlier than listed on ASPACE - is that ok? </t>
         </is>
       </c>
-      <c r="AA88" t="n">
+      <c r="AA88" s="0" t="n">
         <v/>
       </c>
       <c r="AB88" s="103" t="n">
@@ -52764,7 +52764,7 @@
       <c r="Z89" s="68" t="n">
         <v/>
       </c>
-      <c r="AA89" t="n">
+      <c r="AA89" s="0" t="n">
         <v/>
       </c>
       <c r="AB89" s="103" t="n">
@@ -52882,7 +52882,7 @@
       <c r="Z90" s="68" t="n">
         <v/>
       </c>
-      <c r="AA90" t="n">
+      <c r="AA90" s="0" t="n">
         <v/>
       </c>
       <c r="AB90" s="103" t="n">
@@ -53117,7 +53117,7 @@
       <c r="Z92" s="68" t="n">
         <v/>
       </c>
-      <c r="AA92" t="n">
+      <c r="AA92" s="0" t="n">
         <v/>
       </c>
       <c r="AB92" s="103" t="n">
@@ -53233,7 +53233,7 @@
       <c r="Z93" s="68" t="n">
         <v/>
       </c>
-      <c r="AA93" t="n">
+      <c r="AA93" s="0" t="n">
         <v/>
       </c>
       <c r="AB93" s="103" t="n">
@@ -53359,7 +53359,7 @@
           <t>Pass</t>
         </is>
       </c>
-      <c r="AC94" t="n">
+      <c r="AC94" s="0" t="n">
         <v/>
       </c>
       <c r="AD94" s="116" t="n">
@@ -53467,7 +53467,7 @@
       <c r="Z95" s="68" t="n">
         <v/>
       </c>
-      <c r="AA95" t="n">
+      <c r="AA95" s="0" t="n">
         <v/>
       </c>
       <c r="AB95" s="103" t="n">
@@ -53583,7 +53583,7 @@
       <c r="Z96" s="68" t="n">
         <v/>
       </c>
-      <c r="AA96" t="n">
+      <c r="AA96" s="0" t="n">
         <v/>
       </c>
       <c r="AB96" s="103" t="n">
@@ -53699,7 +53699,7 @@
       <c r="Z97" s="68" t="n">
         <v/>
       </c>
-      <c r="AA97" t="n">
+      <c r="AA97" s="0" t="n">
         <v/>
       </c>
       <c r="AB97" s="103" t="n">
@@ -53815,7 +53815,7 @@
       <c r="Z98" s="68" t="n">
         <v/>
       </c>
-      <c r="AA98" t="n">
+      <c r="AA98" s="0" t="n">
         <v/>
       </c>
       <c r="AB98" s="103" t="n">
@@ -53931,7 +53931,7 @@
       <c r="Z99" s="68" t="n">
         <v/>
       </c>
-      <c r="AA99" t="n">
+      <c r="AA99" s="0" t="n">
         <v/>
       </c>
       <c r="AB99" s="103" t="n">
@@ -54047,7 +54047,7 @@
       <c r="Z100" s="68" t="n">
         <v/>
       </c>
-      <c r="AA100" t="n">
+      <c r="AA100" s="0" t="n">
         <v/>
       </c>
       <c r="AB100" s="103" t="n">
@@ -54163,7 +54163,7 @@
       <c r="Z101" s="68" t="n">
         <v/>
       </c>
-      <c r="AA101" t="n">
+      <c r="AA101" s="0" t="n">
         <v/>
       </c>
       <c r="AB101" s="103" t="n">
@@ -54279,7 +54279,7 @@
       <c r="Z102" s="68" t="n">
         <v/>
       </c>
-      <c r="AA102" t="n">
+      <c r="AA102" s="0" t="n">
         <v/>
       </c>
       <c r="AB102" s="103" t="n">
@@ -54391,7 +54391,7 @@
       <c r="Z103" s="68" t="n">
         <v/>
       </c>
-      <c r="AA103" t="n">
+      <c r="AA103" s="0" t="n">
         <v/>
       </c>
       <c r="AB103" s="103" t="n">
@@ -54509,7 +54509,7 @@
           <t xml:space="preserve">Folder says Apparatus but it is a different publication inside </t>
         </is>
       </c>
-      <c r="AA104" t="n">
+      <c r="AA104" s="0" t="n">
         <v/>
       </c>
       <c r="AB104" s="103" t="n">
@@ -54742,7 +54742,7 @@
       <c r="Z106" s="68" t="n">
         <v/>
       </c>
-      <c r="AA106" t="n">
+      <c r="AA106" s="0" t="n">
         <v/>
       </c>
       <c r="AB106" s="103" t="n">
@@ -54860,7 +54860,7 @@
       <c r="Z107" s="68" t="n">
         <v/>
       </c>
-      <c r="AA107" t="n">
+      <c r="AA107" s="0" t="n">
         <v/>
       </c>
       <c r="AB107" s="103" t="n">
@@ -55095,7 +55095,7 @@
           <t xml:space="preserve">GH, MC, JG, SK </t>
         </is>
       </c>
-      <c r="Z109" t="n">
+      <c r="Z109" s="0" t="n">
         <v/>
       </c>
       <c r="AA109" s="103" t="inlineStr">
@@ -59237,7 +59237,7 @@
           <t>QC Pass/Fail</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AD1" s="0" t="inlineStr">
         <is>
           <t>Unnamed: 29</t>
         </is>

</xml_diff>